<commit_message>
Conduct experiments on heuristics
</commit_message>
<xml_diff>
--- a/analysis/experiment_data.xlsx
+++ b/analysis/experiment_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nusu-my.sharepoint.com/personal/e0376997_u_nus_edu/Documents/NUS/Year 3 Sem2/Academics/CS4248/Project/Better-Path/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{A9CE3A51-A5C5-7D42-833E-87A6B4A434BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37B3ECFD-B9CD-D345-A834-77F46913C0A2}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{A9CE3A51-A5C5-7D42-833E-87A6B4A434BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58AB26C7-14CA-A04A-89CA-F7390316D826}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="5980" windowWidth="16660" windowHeight="10360" xr2:uid="{3EF62265-519F-734D-A88B-DAAB2B0B8FD7}"/>
+    <workbookView xWindow="1300" yWindow="5980" windowWidth="16660" windowHeight="10360" activeTab="1" xr2:uid="{3EF62265-519F-734D-A88B-DAAB2B0B8FD7}"/>
   </bookViews>
   <sheets>
     <sheet name="multilayer" sheetId="1" r:id="rId1"/>
+    <sheet name="heuristics" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="141">
   <si>
     <t>iter #</t>
   </si>
@@ -260,6 +261,204 @@
   </si>
   <si>
     <t>hidden layer sizes: 100</t>
+  </si>
+  <si>
+    <t>with heuristics</t>
+  </si>
+  <si>
+    <t>200 test acc: 0.6278975193167955</t>
+  </si>
+  <si>
+    <t>0.4871899145994307</t>
+  </si>
+  <si>
+    <t>0.5124034160227735</t>
+  </si>
+  <si>
+    <t>0.5262301748678324</t>
+  </si>
+  <si>
+    <t>0.5237901586010574</t>
+  </si>
+  <si>
+    <t>0.5685237901586011</t>
+  </si>
+  <si>
+    <t>0.555103700691338</t>
+  </si>
+  <si>
+    <t>0.590890605937373</t>
+  </si>
+  <si>
+    <t>0.6014640097600651</t>
+  </si>
+  <si>
+    <t>0.6136640910939406</t>
+  </si>
+  <si>
+    <t>0.6047173647824319</t>
+  </si>
+  <si>
+    <t>0.6295241968279789</t>
+  </si>
+  <si>
+    <t>0.6287108580723871</t>
+  </si>
+  <si>
+    <t>0.6250508336722245</t>
+  </si>
+  <si>
+    <t>0.6384709231394876</t>
+  </si>
+  <si>
+    <t>0.6270841805612037</t>
+  </si>
+  <si>
+    <t>0.6278975193167955</t>
+  </si>
+  <si>
+    <t>0.6283041886945913</t>
+  </si>
+  <si>
+    <t>0.6437576250508337</t>
+  </si>
+  <si>
+    <t>0.6445709638064254</t>
+  </si>
+  <si>
+    <t>0.6518910126067508</t>
+  </si>
+  <si>
+    <t>* "original" on every page is the best-performing from previous page. Here is multilayer predictor</t>
+  </si>
+  <si>
+    <t>0 test acc: 0.5132167547783651</t>
+  </si>
+  <si>
+    <t>10 test acc: 0.535583570557137</t>
+  </si>
+  <si>
+    <t>20 test acc: 0.5408702724684831</t>
+  </si>
+  <si>
+    <t>30 test acc: 0.5518503456689712</t>
+  </si>
+  <si>
+    <t>40 test acc: 0.5563237088247255</t>
+  </si>
+  <si>
+    <t>50 test acc: 0.5673037820252135</t>
+  </si>
+  <si>
+    <t>60 test acc: 0.5734038226921513</t>
+  </si>
+  <si>
+    <t>70 test acc: 0.5860105734038227</t>
+  </si>
+  <si>
+    <t>80 test acc: 0.588043920292802</t>
+  </si>
+  <si>
+    <t>90 test acc: 0.6201708011386743</t>
+  </si>
+  <si>
+    <t>100 test acc: 0.6274908499389996</t>
+  </si>
+  <si>
+    <t>110 test acc: 0.6287108580723871</t>
+  </si>
+  <si>
+    <t>120 test acc: 0.6384709231394876</t>
+  </si>
+  <si>
+    <t>130 test acc: 0.6258641724278162</t>
+  </si>
+  <si>
+    <t>140 test acc: 0.6091907279381863</t>
+  </si>
+  <si>
+    <t>150 test acc: 0.6425376169174462</t>
+  </si>
+  <si>
+    <t>160 test acc: 0.6283041886945913</t>
+  </si>
+  <si>
+    <t>170 test acc: 0.6392842618950793</t>
+  </si>
+  <si>
+    <t>180 test acc: 0.6457909719398129</t>
+  </si>
+  <si>
+    <t>190 test acc: 0.6417242781618544</t>
+  </si>
+  <si>
+    <t>210 test acc: 0.6421309475396503</t>
+  </si>
+  <si>
+    <t>220 test acc: 0.6514843432289549</t>
+  </si>
+  <si>
+    <t>230 test acc: 0.6494509963399756</t>
+  </si>
+  <si>
+    <t>240 test acc: 0.651077673851159</t>
+  </si>
+  <si>
+    <t>250 test acc: 0.6364375762505083</t>
+  </si>
+  <si>
+    <t>0.5132167547783651</t>
+  </si>
+  <si>
+    <t>0.535583570557137</t>
+  </si>
+  <si>
+    <t>0.5408702724684831</t>
+  </si>
+  <si>
+    <t>0.5518503456689712</t>
+  </si>
+  <si>
+    <t>0.5563237088247255</t>
+  </si>
+  <si>
+    <t>0.5673037820252135</t>
+  </si>
+  <si>
+    <t>0.5734038226921513</t>
+  </si>
+  <si>
+    <t>0.5860105734038227</t>
+  </si>
+  <si>
+    <t>0.588043920292802</t>
+  </si>
+  <si>
+    <t>0.6201708011386743</t>
+  </si>
+  <si>
+    <t>0.6274908499389996</t>
+  </si>
+  <si>
+    <t>0.6258641724278162</t>
+  </si>
+  <si>
+    <t>0.6091907279381863</t>
+  </si>
+  <si>
+    <t>0.6392842618950793</t>
+  </si>
+  <si>
+    <t>0.6417242781618544</t>
+  </si>
+  <si>
+    <t>0.6514843432289549</t>
+  </si>
+  <si>
+    <t>0.6494509963399756</t>
+  </si>
+  <si>
+    <t>0.6364375762505083</t>
   </si>
 </sst>
 </file>
@@ -613,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D228442-1D2C-5941-8A04-C47119D69132}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1036,4 +1235,509 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D3B107-CB91-454C-B64C-5353B8A1C18C}">
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" t="str">
+        <f>RIGHT(G3, LEN(G3)-FIND("/", SUBSTITUTE(G3," ","/", LEN(G3)-LEN(SUBSTITUTE(G3," ","")))))</f>
+        <v>0.5132167547783651</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H28" si="0">RIGHT(G4, LEN(G4)-FIND("/", SUBSTITUTE(G4," ","/", LEN(G4)-LEN(SUBSTITUTE(G4," ","")))))</f>
+        <v>0.535583570557137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>0.5408702724684831</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>0.5518503456689712</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>0.5563237088247255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>0.5673037820252135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>0.5734038226921513</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>0.5860105734038227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>0.588043920292802</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6201708011386743</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" t="s">
+        <v>108</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6274908499389996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6287108580723871</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>130</v>
+      </c>
+      <c r="B15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6384709231394876</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>140</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6258641724278162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>150</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6091907279381863</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>160</v>
+      </c>
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6425376169174462</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>170</v>
+      </c>
+      <c r="B19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6283041886945913</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>180</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6392842618950793</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>190</v>
+      </c>
+      <c r="B21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6457909719398129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>200</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6417242781618544</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>210</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6278975193167955</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>220</v>
+      </c>
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6421309475396503</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>230</v>
+      </c>
+      <c r="B25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" t="s">
+        <v>119</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6514843432289549</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>240</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" t="s">
+        <v>120</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6494509963399756</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>250</v>
+      </c>
+      <c r="B27" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" t="s">
+        <v>121</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="0"/>
+        <v>0.651077673851159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>122</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v>0.6364375762505083</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>